<commit_message>
fixed the dod locations
</commit_message>
<xml_diff>
--- a/2_data_preparation/miscellaneous/dod_area_cost_factors.xlsx
+++ b/2_data_preparation/miscellaneous/dod_area_cost_factors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmendez/Documents/Postdoc/Software_dev/RICE/3_RELOG_simulation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmendez/Documents/Postdoc/Software_dev/RICE/2_data_preparation/miscellaneous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E66F1F42-3EA0-F94B-9DD1-5D7D67E0FFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD97F3BD-30E4-0246-8EB1-EE26D2A65584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="1320" windowWidth="27580" windowHeight="16940" xr2:uid="{B8829C27-7509-684C-A0CB-2E9394D8DECF}"/>
   </bookViews>
@@ -36,7 +36,323 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>State Code</t>
+  </si>
+  <si>
+    <t>ACF Official</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>Washington DC</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>Idaho</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>Mississippi</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>Rhode Island</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>South Dakota</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -385,14 +701,587 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B381A8DA-180D-7348-A9EE-AA38EE55A389}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>